<commit_message>
calculate values per capita using census population
</commit_message>
<xml_diff>
--- a/data/census_state_population.xlsx
+++ b/data/census_state_population.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicho\Development\courses\r\dsba-5122\final_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D6EB46-549A-45CA-A47B-F14C7B223B02}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C2F67B-D065-4316-BF94-ABEB66694F4D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8D4F86FB-8064-483A-A01D-B366D3FE8624}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8D4F86FB-8064-483A-A01D-B366D3FE8624}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -254,14 +254,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -596,17 +592,17 @@
   <dimension ref="A1:J54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -637,1699 +633,1699 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>309326085</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>311580009</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>313874218</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>316057727</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>318386421</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>320742673</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>323071342</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="2">
         <v>325147121</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="2">
         <v>327167434</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>4785448</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>4798834</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>4815564</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>4830460</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>4842481</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>4853160</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <v>4864745</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="2">
         <v>4875120</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="2">
         <v>4887871</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>713906</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>722038</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>730399</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>737045</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>736307</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>737547</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <v>741504</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
         <v>739786</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="2">
         <v>737438</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>6407774</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>6473497</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>6556629</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>6634999</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>6733840</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>6833596</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>6945452</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="2">
         <v>7048876</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="2">
         <v>7171646</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>2921978</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>2940407</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>2952109</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>2959549</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>2967726</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <v>2978407</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <v>2990410</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="2">
         <v>3002997</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="2">
         <v>3013825</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>37320903</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>37641823</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>37960782</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>38280824</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>38625139</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <v>38953142</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <v>39209127</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <v>39399349</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="2">
         <v>39557045</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>5048281</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>5121771</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>5193721</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>5270482</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>5351218</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <v>5452107</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="2">
         <v>5540921</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="2">
         <v>5615902</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="2">
         <v>5695564</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>3579125</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>3588023</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>3594395</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>3594915</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>3594783</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <v>3587509</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <v>3578674</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="2">
         <v>3573880</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="2">
         <v>3572665</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>899595</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>907316</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>915188</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>923638</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>932596</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <v>941413</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="2">
         <v>949216</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="2">
         <v>957078</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="2">
         <v>967171</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>605085</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>619602</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>634725</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>650431</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <v>662513</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="2">
         <v>675254</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="2">
         <v>686575</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="2">
         <v>695691</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="2">
         <v>702455</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>18845785</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>19093352</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>19326230</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>19563166</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <v>19860330</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="2">
         <v>20224249</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="2">
         <v>20629982</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="2">
         <v>20976812</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="2">
         <v>21299325</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>9711810</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>9801578</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>9901496</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <v>9973326</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="2">
         <v>10069001</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="2">
         <v>10181111</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="2">
         <v>10304763</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13" s="2">
         <v>10413055</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13" s="2">
         <v>10519475</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>1363963</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>1379252</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>1394905</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <v>1408453</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="2">
         <v>1414862</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="2">
         <v>1422484</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="2">
         <v>1428105</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="2">
         <v>1424203</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="2">
         <v>1420491</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>1570773</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>1583828</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <v>1595441</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <v>1611530</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="2">
         <v>1631479</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="2">
         <v>1651523</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="2">
         <v>1682930</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15" s="2">
         <v>1718904</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="2">
         <v>1754208</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>12840762</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <v>12867291</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="2">
         <v>12884119</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <v>12898269</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="2">
         <v>12888962</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="2">
         <v>12864342</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="2">
         <v>12826895</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I16" s="2">
         <v>12786196</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="2">
         <v>12741080</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>6490436</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>6516045</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <v>6537640</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="2">
         <v>6568367</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="2">
         <v>6593533</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="2">
         <v>6608296</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="2">
         <v>6633344</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I17" s="2">
         <v>6660082</v>
       </c>
-      <c r="J17" s="3">
+      <c r="J17" s="2">
         <v>6691878</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>3050767</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>3066054</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="2">
         <v>3076097</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="2">
         <v>3093078</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="2">
         <v>3109504</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18" s="2">
         <v>3121460</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="2">
         <v>3131785</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18" s="2">
         <v>3143637</v>
       </c>
-      <c r="J18" s="3">
+      <c r="J18" s="2">
         <v>3156145</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="2">
         <v>2858213</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>2869035</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="2">
         <v>2885361</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="2">
         <v>2893510</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="2">
         <v>2900896</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="2">
         <v>2909502</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="2">
         <v>2911263</v>
       </c>
-      <c r="I19" s="3">
+      <c r="I19" s="2">
         <v>2910689</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J19" s="2">
         <v>2911505</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="2">
         <v>4348200</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="2">
         <v>4369488</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="2">
         <v>4386381</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <v>4404817</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="2">
         <v>4414483</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="2">
         <v>4425999</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="2">
         <v>4438229</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I20" s="2">
         <v>4453874</v>
       </c>
-      <c r="J20" s="3">
+      <c r="J20" s="2">
         <v>4468402</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="2">
         <v>4544532</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="2">
         <v>4575184</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="2">
         <v>4600814</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="2">
         <v>4624577</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="2">
         <v>4644204</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="2">
         <v>4664851</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="2">
         <v>4678215</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21" s="2">
         <v>4670818</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J21" s="2">
         <v>4659978</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>1327632</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <v>1328150</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="2">
         <v>1327691</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <v>1328196</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="2">
         <v>1330760</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G22" s="2">
         <v>1328484</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="2">
         <v>1331370</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22" s="2">
         <v>1335063</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J22" s="2">
         <v>1338404</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <v>5788642</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>5838991</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="2">
         <v>5887072</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <v>5923704</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="2">
         <v>5958165</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23" s="2">
         <v>5986717</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="2">
         <v>6004692</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23" s="2">
         <v>6024891</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J23" s="2">
         <v>6042718</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <v>6566431</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <v>6613149</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="2">
         <v>6663158</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="2">
         <v>6713944</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="2">
         <v>6763652</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G24" s="2">
         <v>6795891</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24" s="2">
         <v>6826022</v>
       </c>
-      <c r="I24" s="3">
+      <c r="I24" s="2">
         <v>6863246</v>
       </c>
-      <c r="J24" s="3">
+      <c r="J24" s="2">
         <v>6902149</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="2">
         <v>9877535</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="2">
         <v>9881521</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="2">
         <v>9896930</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="2">
         <v>9913349</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="2">
         <v>9930589</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G25" s="2">
         <v>9932573</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25" s="2">
         <v>9951890</v>
       </c>
-      <c r="I25" s="3">
+      <c r="I25" s="2">
         <v>9976447</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J25" s="2">
         <v>9995915</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="2">
         <v>5310843</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="2">
         <v>5345668</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="2">
         <v>5376550</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="2">
         <v>5413693</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="2">
         <v>5451522</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G26" s="2">
         <v>5482503</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H26" s="2">
         <v>5523409</v>
       </c>
-      <c r="I26" s="3">
+      <c r="I26" s="2">
         <v>5568155</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J26" s="2">
         <v>5611179</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="2">
         <v>2970536</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="2">
         <v>2978470</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="2">
         <v>2983767</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="2">
         <v>2988797</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="2">
         <v>2990623</v>
       </c>
-      <c r="G27" s="3">
+      <c r="G27" s="2">
         <v>2988693</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H27" s="2">
         <v>2988298</v>
       </c>
-      <c r="I27" s="3">
+      <c r="I27" s="2">
         <v>2989663</v>
       </c>
-      <c r="J27" s="3">
+      <c r="J27" s="2">
         <v>2986530</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="2">
         <v>5995976</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="2">
         <v>6009641</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="2">
         <v>6024081</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="2">
         <v>6040658</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="2">
         <v>6056293</v>
       </c>
-      <c r="G28" s="3">
+      <c r="G28" s="2">
         <v>6071745</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H28" s="2">
         <v>6087203</v>
       </c>
-      <c r="I28" s="3">
+      <c r="I28" s="2">
         <v>6108612</v>
       </c>
-      <c r="J28" s="3">
+      <c r="J28" s="2">
         <v>6126452</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="2">
         <v>990722</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="2">
         <v>997221</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="2">
         <v>1003754</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="2">
         <v>1013564</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29" s="2">
         <v>1021891</v>
       </c>
-      <c r="G29" s="3">
+      <c r="G29" s="2">
         <v>1030503</v>
       </c>
-      <c r="H29" s="3">
+      <c r="H29" s="2">
         <v>1040863</v>
       </c>
-      <c r="I29" s="3">
+      <c r="I29" s="2">
         <v>1053090</v>
       </c>
-      <c r="J29" s="3">
+      <c r="J29" s="2">
         <v>1062305</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="2">
         <v>1829536</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="2">
         <v>1840538</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="2">
         <v>1853323</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="2">
         <v>1865414</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30" s="2">
         <v>1879522</v>
       </c>
-      <c r="G30" s="3">
+      <c r="G30" s="2">
         <v>1891507</v>
       </c>
-      <c r="H30" s="3">
+      <c r="H30" s="2">
         <v>1905924</v>
       </c>
-      <c r="I30" s="3">
+      <c r="I30" s="2">
         <v>1917575</v>
       </c>
-      <c r="J30" s="3">
+      <c r="J30" s="2">
         <v>1929268</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="2">
         <v>2702464</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="2">
         <v>2712799</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="2">
         <v>2744566</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="2">
         <v>2776972</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F31" s="2">
         <v>2819012</v>
       </c>
-      <c r="G31" s="3">
+      <c r="G31" s="2">
         <v>2868666</v>
       </c>
-      <c r="H31" s="3">
+      <c r="H31" s="2">
         <v>2919772</v>
       </c>
-      <c r="I31" s="3">
+      <c r="I31" s="2">
         <v>2972405</v>
       </c>
-      <c r="J31" s="3">
+      <c r="J31" s="2">
         <v>3034392</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="2">
         <v>1316777</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="2">
         <v>1319815</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="2">
         <v>1323962</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="2">
         <v>1326408</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F32" s="2">
         <v>1333223</v>
       </c>
-      <c r="G32" s="3">
+      <c r="G32" s="2">
         <v>1336294</v>
       </c>
-      <c r="H32" s="3">
+      <c r="H32" s="2">
         <v>1342373</v>
       </c>
-      <c r="I32" s="3">
+      <c r="I32" s="2">
         <v>1349767</v>
       </c>
-      <c r="J32" s="3">
+      <c r="J32" s="2">
         <v>1356458</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="2">
         <v>8799624</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="2">
         <v>8827783</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="2">
         <v>8845483</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33" s="2">
         <v>8858362</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F33" s="2">
         <v>8866780</v>
       </c>
-      <c r="G33" s="3">
+      <c r="G33" s="2">
         <v>8870869</v>
       </c>
-      <c r="H33" s="3">
+      <c r="H33" s="2">
         <v>8874516</v>
       </c>
-      <c r="I33" s="3">
+      <c r="I33" s="2">
         <v>8888543</v>
       </c>
-      <c r="J33" s="3">
+      <c r="J33" s="2">
         <v>8908520</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="2">
         <v>2064588</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="2">
         <v>2080395</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="2">
         <v>2087549</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34" s="2">
         <v>2092792</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F34" s="2">
         <v>2090342</v>
       </c>
-      <c r="G34" s="3">
+      <c r="G34" s="2">
         <v>2090211</v>
       </c>
-      <c r="H34" s="3">
+      <c r="H34" s="2">
         <v>2092789</v>
       </c>
-      <c r="I34" s="3">
+      <c r="I34" s="2">
         <v>2093395</v>
       </c>
-      <c r="J34" s="3">
+      <c r="J34" s="2">
         <v>2095428</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="2">
         <v>19400080</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="2">
         <v>19498514</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="2">
         <v>19574549</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E35" s="2">
         <v>19628043</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F35" s="2">
         <v>19656330</v>
       </c>
-      <c r="G35" s="3">
+      <c r="G35" s="2">
         <v>19661411</v>
       </c>
-      <c r="H35" s="3">
+      <c r="H35" s="2">
         <v>19641589</v>
       </c>
-      <c r="I35" s="3">
+      <c r="I35" s="2">
         <v>19590719</v>
       </c>
-      <c r="J35" s="3">
+      <c r="J35" s="2">
         <v>19542209</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="2">
         <v>9574293</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36" s="2">
         <v>9656754</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="2">
         <v>9749123</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36" s="2">
         <v>9843599</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F36" s="2">
         <v>9933944</v>
       </c>
-      <c r="G36" s="3">
+      <c r="G36" s="2">
         <v>10033079</v>
       </c>
-      <c r="H36" s="3">
+      <c r="H36" s="2">
         <v>10156679</v>
       </c>
-      <c r="I36" s="3">
+      <c r="I36" s="2">
         <v>10270800</v>
       </c>
-      <c r="J36" s="3">
+      <c r="J36" s="2">
         <v>10383620</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="2">
         <v>674710</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37" s="2">
         <v>685136</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="2">
         <v>701116</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E37" s="2">
         <v>721999</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F37" s="2">
         <v>737382</v>
       </c>
-      <c r="G37" s="3">
+      <c r="G37" s="2">
         <v>754022</v>
       </c>
-      <c r="H37" s="3">
+      <c r="H37" s="2">
         <v>754353</v>
       </c>
-      <c r="I37" s="3">
+      <c r="I37" s="2">
         <v>755176</v>
       </c>
-      <c r="J37" s="3">
+      <c r="J37" s="2">
         <v>760077</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="2">
         <v>11539327</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="2">
         <v>11543463</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38" s="2">
         <v>11548369</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E38" s="2">
         <v>11576576</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F38" s="2">
         <v>11602973</v>
       </c>
-      <c r="G38" s="3">
+      <c r="G38" s="2">
         <v>11617850</v>
       </c>
-      <c r="H38" s="3">
+      <c r="H38" s="2">
         <v>11635003</v>
       </c>
-      <c r="I38" s="3">
+      <c r="I38" s="2">
         <v>11664129</v>
       </c>
-      <c r="J38" s="3">
+      <c r="J38" s="2">
         <v>11689442</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="2">
         <v>3759632</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39" s="2">
         <v>3787821</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="2">
         <v>3818600</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E39" s="2">
         <v>3853205</v>
       </c>
-      <c r="F39" s="3">
+      <c r="F39" s="2">
         <v>3878367</v>
       </c>
-      <c r="G39" s="3">
+      <c r="G39" s="2">
         <v>3909831</v>
       </c>
-      <c r="H39" s="3">
+      <c r="H39" s="2">
         <v>3926769</v>
       </c>
-      <c r="I39" s="3">
+      <c r="I39" s="2">
         <v>3932640</v>
       </c>
-      <c r="J39" s="3">
+      <c r="J39" s="2">
         <v>3943079</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="2">
         <v>3837532</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40" s="2">
         <v>3871728</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="2">
         <v>3899118</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E40" s="2">
         <v>3922908</v>
       </c>
-      <c r="F40" s="3">
+      <c r="F40" s="2">
         <v>3964106</v>
       </c>
-      <c r="G40" s="3">
+      <c r="G40" s="2">
         <v>4016918</v>
       </c>
-      <c r="H40" s="3">
+      <c r="H40" s="2">
         <v>4091404</v>
       </c>
-      <c r="I40" s="3">
+      <c r="I40" s="2">
         <v>4146592</v>
       </c>
-      <c r="J40" s="3">
+      <c r="J40" s="2">
         <v>4190713</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41" s="2">
         <v>12711158</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C41" s="2">
         <v>12744583</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41" s="2">
         <v>12766827</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E41" s="2">
         <v>12776621</v>
       </c>
-      <c r="F41" s="3">
+      <c r="F41" s="2">
         <v>12789101</v>
       </c>
-      <c r="G41" s="3">
+      <c r="G41" s="2">
         <v>12785759</v>
       </c>
-      <c r="H41" s="3">
+      <c r="H41" s="2">
         <v>12783538</v>
       </c>
-      <c r="I41" s="3">
+      <c r="I41" s="2">
         <v>12790447</v>
       </c>
-      <c r="J41" s="3">
+      <c r="J41" s="2">
         <v>12807060</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="2">
         <v>1053938</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C42" s="2">
         <v>1053536</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="2">
         <v>1054601</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E42" s="2">
         <v>1055122</v>
       </c>
-      <c r="F42" s="3">
+      <c r="F42" s="2">
         <v>1056017</v>
       </c>
-      <c r="G42" s="3">
+      <c r="G42" s="2">
         <v>1056173</v>
       </c>
-      <c r="H42" s="3">
+      <c r="H42" s="2">
         <v>1057063</v>
       </c>
-      <c r="I42" s="3">
+      <c r="I42" s="2">
         <v>1056486</v>
       </c>
-      <c r="J42" s="3">
+      <c r="J42" s="2">
         <v>1057315</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43" s="2">
         <v>4635656</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43" s="2">
         <v>4671422</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="2">
         <v>4717112</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E43" s="2">
         <v>4764153</v>
       </c>
-      <c r="F43" s="3">
+      <c r="F43" s="2">
         <v>4823793</v>
       </c>
-      <c r="G43" s="3">
+      <c r="G43" s="2">
         <v>4892253</v>
       </c>
-      <c r="H43" s="3">
+      <c r="H43" s="2">
         <v>4958235</v>
       </c>
-      <c r="I43" s="3">
+      <c r="I43" s="2">
         <v>5021219</v>
       </c>
-      <c r="J43" s="3">
+      <c r="J43" s="2">
         <v>5084127</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="2">
         <v>816165</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C44" s="2">
         <v>823484</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44" s="2">
         <v>833496</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E44" s="2">
         <v>842270</v>
       </c>
-      <c r="F44" s="3">
+      <c r="F44" s="2">
         <v>849088</v>
       </c>
-      <c r="G44" s="3">
+      <c r="G44" s="2">
         <v>853933</v>
       </c>
-      <c r="H44" s="3">
+      <c r="H44" s="2">
         <v>862890</v>
       </c>
-      <c r="I44" s="3">
+      <c r="I44" s="2">
         <v>873286</v>
       </c>
-      <c r="J44" s="3">
+      <c r="J44" s="2">
         <v>882235</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45" s="2">
         <v>6355301</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45" s="2">
         <v>6397410</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45" s="2">
         <v>6451281</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45" s="2">
         <v>6493432</v>
       </c>
-      <c r="F45" s="3">
+      <c r="F45" s="2">
         <v>6540826</v>
       </c>
-      <c r="G45" s="3">
+      <c r="G45" s="2">
         <v>6590808</v>
       </c>
-      <c r="H45" s="3">
+      <c r="H45" s="2">
         <v>6645011</v>
       </c>
-      <c r="I45" s="3">
+      <c r="I45" s="2">
         <v>6708794</v>
       </c>
-      <c r="J45" s="3">
+      <c r="J45" s="2">
         <v>6770010</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46" s="2">
         <v>25242679</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C46" s="2">
         <v>25646227</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D46" s="2">
         <v>26089620</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E46" s="2">
         <v>26489464</v>
       </c>
-      <c r="F46" s="3">
+      <c r="F46" s="2">
         <v>26977142</v>
       </c>
-      <c r="G46" s="3">
+      <c r="G46" s="2">
         <v>27486814</v>
       </c>
-      <c r="H46" s="3">
+      <c r="H46" s="2">
         <v>27937492</v>
       </c>
-      <c r="I46" s="3">
+      <c r="I46" s="2">
         <v>28322717</v>
       </c>
-      <c r="J46" s="3">
+      <c r="J46" s="2">
         <v>28701845</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="2">
         <v>2775334</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C47" s="2">
         <v>2814216</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D47" s="2">
         <v>2853467</v>
       </c>
-      <c r="E47" s="3">
+      <c r="E47" s="2">
         <v>2897927</v>
       </c>
-      <c r="F47" s="3">
+      <c r="F47" s="2">
         <v>2937399</v>
       </c>
-      <c r="G47" s="3">
+      <c r="G47" s="2">
         <v>2982497</v>
       </c>
-      <c r="H47" s="3">
+      <c r="H47" s="2">
         <v>3042613</v>
       </c>
-      <c r="I47" s="3">
+      <c r="I47" s="2">
         <v>3103118</v>
       </c>
-      <c r="J47" s="3">
+      <c r="J47" s="2">
         <v>3161105</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="2">
         <v>625880</v>
       </c>
-      <c r="C48" s="3">
+      <c r="C48" s="2">
         <v>626979</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D48" s="2">
         <v>626063</v>
       </c>
-      <c r="E48" s="3">
+      <c r="E48" s="2">
         <v>626212</v>
       </c>
-      <c r="F48" s="3">
+      <c r="F48" s="2">
         <v>625218</v>
       </c>
-      <c r="G48" s="3">
+      <c r="G48" s="2">
         <v>625197</v>
       </c>
-      <c r="H48" s="3">
+      <c r="H48" s="2">
         <v>623644</v>
       </c>
-      <c r="I48" s="3">
+      <c r="I48" s="2">
         <v>624525</v>
       </c>
-      <c r="J48" s="3">
+      <c r="J48" s="2">
         <v>626299</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="2">
         <v>8023680</v>
       </c>
-      <c r="C49" s="3">
+      <c r="C49" s="2">
         <v>8100469</v>
       </c>
-      <c r="D49" s="3">
+      <c r="D49" s="2">
         <v>8185229</v>
       </c>
-      <c r="E49" s="3">
+      <c r="E49" s="2">
         <v>8253053</v>
       </c>
-      <c r="F49" s="3">
+      <c r="F49" s="2">
         <v>8312076</v>
       </c>
-      <c r="G49" s="3">
+      <c r="G49" s="2">
         <v>8362907</v>
       </c>
-      <c r="H49" s="3">
+      <c r="H49" s="2">
         <v>8410946</v>
       </c>
-      <c r="I49" s="3">
+      <c r="I49" s="2">
         <v>8465207</v>
       </c>
-      <c r="J49" s="3">
+      <c r="J49" s="2">
         <v>8517685</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B50" s="2">
         <v>6742902</v>
       </c>
-      <c r="C50" s="3">
+      <c r="C50" s="2">
         <v>6821655</v>
       </c>
-      <c r="D50" s="3">
+      <c r="D50" s="2">
         <v>6892876</v>
       </c>
-      <c r="E50" s="3">
+      <c r="E50" s="2">
         <v>6962906</v>
       </c>
-      <c r="F50" s="3">
+      <c r="F50" s="2">
         <v>7052439</v>
       </c>
-      <c r="G50" s="3">
+      <c r="G50" s="2">
         <v>7163543</v>
       </c>
-      <c r="H50" s="3">
+      <c r="H50" s="2">
         <v>7294680</v>
       </c>
-      <c r="I50" s="3">
+      <c r="I50" s="2">
         <v>7425432</v>
       </c>
-      <c r="J50" s="3">
+      <c r="J50" s="2">
         <v>7535591</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B51" s="2">
         <v>1854214</v>
       </c>
-      <c r="C51" s="3">
+      <c r="C51" s="2">
         <v>1856074</v>
       </c>
-      <c r="D51" s="3">
+      <c r="D51" s="2">
         <v>1856764</v>
       </c>
-      <c r="E51" s="3">
+      <c r="E51" s="2">
         <v>1853873</v>
       </c>
-      <c r="F51" s="3">
+      <c r="F51" s="2">
         <v>1849467</v>
       </c>
-      <c r="G51" s="3">
+      <c r="G51" s="2">
         <v>1841996</v>
       </c>
-      <c r="H51" s="3">
+      <c r="H51" s="2">
         <v>1830929</v>
       </c>
-      <c r="I51" s="3">
+      <c r="I51" s="2">
         <v>1817048</v>
       </c>
-      <c r="J51" s="3">
+      <c r="J51" s="2">
         <v>1805832</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B52" s="3">
+      <c r="B52" s="2">
         <v>5690479</v>
       </c>
-      <c r="C52" s="3">
+      <c r="C52" s="2">
         <v>5704755</v>
       </c>
-      <c r="D52" s="3">
+      <c r="D52" s="2">
         <v>5719855</v>
       </c>
-      <c r="E52" s="3">
+      <c r="E52" s="2">
         <v>5736952</v>
       </c>
-      <c r="F52" s="3">
+      <c r="F52" s="2">
         <v>5751974</v>
       </c>
-      <c r="G52" s="3">
+      <c r="G52" s="2">
         <v>5761406</v>
       </c>
-      <c r="H52" s="3">
+      <c r="H52" s="2">
         <v>5772958</v>
       </c>
-      <c r="I52" s="3">
+      <c r="I52" s="2">
         <v>5792051</v>
       </c>
-      <c r="J52" s="3">
+      <c r="J52" s="2">
         <v>5813568</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B53" s="3">
+      <c r="B53" s="2">
         <v>564483</v>
       </c>
-      <c r="C53" s="3">
+      <c r="C53" s="2">
         <v>567224</v>
       </c>
-      <c r="D53" s="3">
+      <c r="D53" s="2">
         <v>576270</v>
       </c>
-      <c r="E53" s="3">
+      <c r="E53" s="2">
         <v>582123</v>
       </c>
-      <c r="F53" s="3">
+      <c r="F53" s="2">
         <v>582548</v>
       </c>
-      <c r="G53" s="3">
+      <c r="G53" s="2">
         <v>585668</v>
       </c>
-      <c r="H53" s="3">
+      <c r="H53" s="2">
         <v>584290</v>
       </c>
-      <c r="I53" s="3">
+      <c r="I53" s="2">
         <v>578934</v>
       </c>
-      <c r="J53" s="3">
+      <c r="J53" s="2">
         <v>577737</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B54" s="3">
+      <c r="B54" s="2">
         <v>3721525</v>
       </c>
-      <c r="C54" s="3">
+      <c r="C54" s="2">
         <v>3678732</v>
       </c>
-      <c r="D54" s="3">
+      <c r="D54" s="2">
         <v>3634488</v>
       </c>
-      <c r="E54" s="3">
+      <c r="E54" s="2">
         <v>3593077</v>
       </c>
-      <c r="F54" s="3">
+      <c r="F54" s="2">
         <v>3534874</v>
       </c>
-      <c r="G54" s="3">
+      <c r="G54" s="2">
         <v>3473166</v>
       </c>
-      <c r="H54" s="3">
+      <c r="H54" s="2">
         <v>3406495</v>
       </c>
-      <c r="I54" s="3">
+      <c r="I54" s="2">
         <v>3325001</v>
       </c>
-      <c r="J54" s="3">
+      <c r="J54" s="2">
         <v>3195153</v>
       </c>
     </row>

</xml_diff>